<commit_message>
added support for data and time inputs
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects and porfolio\Projects\self\R Shiny Survey Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC9C495-154C-43C7-BA96-C5C42521FEC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE56F4BA-71F0-4939-A8C4-7BEE1B61014D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="3195" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Module</t>
   </si>
@@ -90,10 +90,13 @@
     <t>Pick a date</t>
   </si>
   <si>
-    <t>Pick a time</t>
-  </si>
-  <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>2020-01-01,2020-12-31</t>
+  </si>
+  <si>
+    <t>Pick a time (24 hrs)</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,6 +513,9 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -521,16 +527,19 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added support for specifying min max and default value for numeric input
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects and porfolio\Projects\self\R Shiny Survey Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE56F4BA-71F0-4939-A8C4-7BEE1B61014D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD9A904-81CD-4AB1-AAFB-4821733096C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="3195" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Module</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Pick a time (24 hrs)</t>
+  </si>
+  <si>
+    <t>1,27,3</t>
+  </si>
+  <si>
+    <t>1,100,20</t>
   </si>
 </sst>
 </file>
@@ -417,7 +423,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,6 +472,9 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -476,6 +485,9 @@
       </c>
       <c r="C4" t="s">
         <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>